<commit_message>
Refactor the code in Game & PlayerObject
</commit_message>
<xml_diff>
--- a/Project plan.xlsx
+++ b/Project plan.xlsx
@@ -449,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -458,7 +458,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,8 +480,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +801,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,322 +835,322 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="F3" s="10"/>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="F4" s="15"/>
+      <c r="B4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="F5" s="16"/>
+      <c r="B5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="F6" s="16"/>
+      <c r="B6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="F7" s="16"/>
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="F8" s="16"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="F9" s="16"/>
+      <c r="B9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="F10" s="16"/>
+      <c r="B10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="F11" s="16"/>
+      <c r="A11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="F12" s="16"/>
+      <c r="A12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="F13" s="16"/>
+      <c r="A13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="F14" s="16"/>
+      <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="F15" s="16"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="F16" s="16"/>
+      <c r="A16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="F17" s="16"/>
+      <c r="A17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="F18" s="16"/>
+      <c r="A18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="F19" s="16"/>
+      <c r="A19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="F20" s="16"/>
+      <c r="A20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="F21" s="16"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="F22" s="16"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="13"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="F23" s="16"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="F24" s="16"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="F25" s="16"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="13"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="F26" s="16"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="13"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="F27" s="16"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="13"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="F28" s="16"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="13"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="F29" s="16"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="16"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="14"/>
-      <c r="F31" s="16"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="F32" s="16"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="16"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="14"/>
-      <c r="F34" s="16"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="F35" s="16"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="F36" s="16"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="13"/>
+      <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="14"/>
-      <c r="F37" s="16"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="13"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="14"/>
-      <c r="F38" s="16"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>

</xml_diff>